<commit_message>
assess OPN logistic regression on essays&myPersonality
</commit_message>
<xml_diff>
--- a/analysis/llm-dataset-generation/traits-definitions.xlsx
+++ b/analysis/llm-dataset-generation/traits-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliran/Personal/dev/Musical-Preferences-And-Textual-Expression/analysis/llm-dataset-generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4C37F-01B7-8C4F-9933-94B7C573E64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4323300-7BDF-314E-8254-BB0C2D9ED8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="760" windowWidth="30220" windowHeight="21580" activeTab="7" xr2:uid="{E88F0C86-A023-0E47-8DEA-32C7060B808F}"/>
+    <workbookView xWindow="42580" yWindow="500" windowWidth="30220" windowHeight="21100" firstSheet="2" activeTab="4" xr2:uid="{E88F0C86-A023-0E47-8DEA-32C7060B808F}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="Low-Openness-Bard" sheetId="11" r:id="rId5"/>
     <sheet name="Openness-GPT3.5" sheetId="3" r:id="rId6"/>
     <sheet name="High-Openness-GPT3.5" sheetId="7" r:id="rId7"/>
-    <sheet name="Low-Openness-GPT3.5" sheetId="8" r:id="rId8"/>
-    <sheet name="Openness-Bing-GPT4" sheetId="4" r:id="rId9"/>
+    <sheet name="Low-openness classifier verifi" sheetId="12" r:id="rId8"/>
+    <sheet name="Low-Openness-GPT3.5" sheetId="8" r:id="rId9"/>
+    <sheet name="Openness-Bing-GPT4" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="agreeableness" localSheetId="0">Definitions!$B$39</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="1079">
   <si>
     <t>Openness (also referred to as openness to experience) emphasizes imagination and insight the most out of all five personality traits. People who are high in openness tend to have a broad range of interests. They are curious about the world and other people and are eager to learn new things and enjoy new experiences. People who are high in this personality trait also tend to be more adventurous and creative. Conversely, people low in this personality trait are often much more traditional and may struggle with abstract thinking.</t>
   </si>
@@ -3256,6 +3257,48 @@
   </si>
   <si>
     <t>The bookstore shelves stretched into the distance, an ocean of spines promising countless adventures. My friends excitedly dug through dusty tomes, their fingers trailing across leather covers. But to me, the sheer volume was overwhelming, the endless choices paralyzing. I reached for my well-worn copy of Harry Potter, its tattered pages holding a world I knew like the back</t>
+  </si>
+  <si>
+    <t>In the quiet simplicity of my daily routine, I find comfort and stability. The predictability of each day allows me to focus on the tasks at hand without the distractions of constant change. I appreciate the familiar patterns that guide my actions, providing a sense of order in a world that can often be chaotic.</t>
+  </si>
+  <si>
+    <t>Change has always been a source of discomfort for me. Whether it's a new technology or a different way of doing things, I prefer the tried and true. Routines offer a sense of security, a sanctuary where I can navigate life with confidence. The unfamiliarity of change tends to stir a sense of unease within me.</t>
+  </si>
+  <si>
+    <t>I've never been one to seek out exotic experiences or adventurous endeavors. The thought of traveling to distant lands and immersing myself in unfamiliar cultures doesn't hold the same allure as the comfort of my own home. I find solace in the familiar surroundings that reflect the stability I value.</t>
+  </si>
+  <si>
+    <t>Abstract concepts and theoretical ideas often elude my grasp. I appreciate practicality and straightforward thinking. The complexities of abstract thought can feel overwhelming and unnecessary, as I prefer to focus on tangible and concrete solutions to problems that arise.</t>
+  </si>
+  <si>
+    <t>Creativity has never been my strong suit. I find satisfaction in the execution of established methods rather than exploring innovative approaches. While others may revel in the realm of imagination, I am content with the proven and practical, steering clear of the unpredictable.</t>
+  </si>
+  <si>
+    <t>Routine and predictability define my comfort zone. The thought of stepping into the unknown triggers a sense of anxiety. I thrive in environments where expectations are clear, and deviations from the norm are kept to a minimum. Stability is my compass in the journey of life.</t>
+  </si>
+  <si>
+    <t>Immersing myself in diverse interests has never been a priority. I find contentment in the familiarity of a select few hobbies that resonate with my grounded nature. The idea of cultivating an extensive range of interests seems unnecessary when my existing pursuits bring me fulfillment.</t>
+  </si>
+  <si>
+    <t>While others may relish the excitement of tackling new challenges, I find satisfaction in mastering the familiar. The prospect of constant change and the need for adaptation seem daunting, and I prefer the steadiness of a well-trodden path.</t>
+  </si>
+  <si>
+    <t>The prospect of embracing unconventional ideas or unconventional approaches leaves me skeptical. I hold a preference for traditions that have stood the test of time, finding comfort in the wisdom of tried-and-true practices. Novelty may have its appeal, but stability remains my anchor.</t>
+  </si>
+  <si>
+    <t>In a world that often celebrates the open-minded and adventurous, I find solace in the reliability of closedness. The known provides a sanctuary where I can navigate life with confidence, free from the uncertainties that accompany a more open approach.</t>
+  </si>
+  <si>
+    <t>The paragraphs above were generated by ChatGPT3.5, as texts written by writters with low openness.</t>
+  </si>
+  <si>
+    <t>This is done as part of a small experiment to verify that Bard's generated texts repeated paragraph-patterns too often, which we estimate caused the model trained on Bard's data to overfit these patterns.</t>
+  </si>
+  <si>
+    <t>To verify this, we simply created a small set of 10 paragraphs, written by writters with low openness. To this set we will append the repeating prefix: "aren't just"</t>
+  </si>
+  <si>
+    <t>Then, we'll ask the model trained on Bard's data to classify: high vs low openness. We assume that the prefix addition will make it mistake and predict LOW, wrongly.</t>
   </si>
 </sst>
 </file>
@@ -3530,6 +3573,42 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3557,15 +3636,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3574,33 +3644,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3930,7 +3973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A05D79-292C-0B47-977C-AC2DE08B5B40}">
   <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -3962,7 +4005,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="32" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -3979,8 +4022,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="47"/>
-      <c r="B3" s="38"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="11"/>
       <c r="D3" s="9" t="s">
         <v>1</v>
@@ -3990,8 +4033,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="39"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="11"/>
       <c r="D4" s="9" t="s">
         <v>2</v>
@@ -4001,8 +4044,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="11"/>
       <c r="D5" s="9" t="s">
         <v>3</v>
@@ -4012,8 +4055,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="11"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
@@ -4021,7 +4064,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="17" t="s">
         <v>24</v>
       </c>
@@ -4036,8 +4079,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
-      <c r="B8" s="51"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="17"/>
       <c r="D8" s="7" t="s">
         <v>16</v>
@@ -4047,8 +4090,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="17"/>
       <c r="D9" s="7" t="s">
         <v>17</v>
@@ -4058,8 +4101,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="17"/>
       <c r="D10" s="7" t="s">
         <v>18</v>
@@ -4069,8 +4112,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="47"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="17"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
@@ -4078,7 +4121,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="20" t="s">
         <v>39</v>
       </c>
@@ -4093,8 +4136,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="18"/>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -4104,8 +4147,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="18"/>
       <c r="D14" s="5" t="s">
         <v>28</v>
@@ -4115,8 +4158,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="18"/>
       <c r="D15" s="5" t="s">
         <v>29</v>
@@ -4126,8 +4169,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="18"/>
       <c r="D16" s="5" t="s">
         <v>30</v>
@@ -4137,8 +4180,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="47"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="18"/>
       <c r="D17" s="5" t="s">
         <v>31</v>
@@ -4148,8 +4191,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="18"/>
       <c r="D18" s="5" t="s">
         <v>32</v>
@@ -4157,7 +4200,7 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="19" t="s">
         <v>51</v>
       </c>
@@ -4172,8 +4215,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="47"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="19"/>
       <c r="D20" s="6" t="s">
         <v>42</v>
@@ -4183,8 +4226,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="47"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="19"/>
       <c r="D21" s="6" t="s">
         <v>43</v>
@@ -4194,8 +4237,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="47"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="19"/>
       <c r="D22" s="6" t="s">
         <v>44</v>
@@ -4205,8 +4248,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="47"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="19"/>
       <c r="D23" s="6" t="s">
         <v>45</v>
@@ -4216,7 +4259,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="47"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="13" t="s">
         <v>65</v>
       </c>
@@ -4231,8 +4274,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="47"/>
-      <c r="B25" s="44"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="14"/>
       <c r="D25" s="8" t="s">
         <v>54</v>
@@ -4242,8 +4285,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="47"/>
-      <c r="B26" s="45"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="15"/>
       <c r="D26" s="8" t="s">
         <v>55</v>
@@ -4253,8 +4296,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="47"/>
-      <c r="B27" s="45"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="15"/>
       <c r="D27" s="8" t="s">
         <v>56</v>
@@ -4264,8 +4307,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="47"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="15"/>
       <c r="D28" s="8" t="s">
         <v>57</v>
@@ -4275,8 +4318,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="47"/>
-      <c r="B29" s="46"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="16"/>
       <c r="D29" s="8" t="s">
         <v>58</v>
@@ -4301,7 +4344,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="33" t="s">
         <v>155</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -4318,8 +4361,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="47"/>
-      <c r="B32" s="32"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
         <v>81</v>
@@ -4329,8 +4372,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="47"/>
-      <c r="B33" s="33"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5" t="s">
         <v>82</v>
@@ -4340,8 +4383,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="47"/>
-      <c r="B34" s="33"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5" t="s">
         <v>83</v>
@@ -4351,8 +4394,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="47"/>
-      <c r="B35" s="33"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="45"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
         <v>84</v>
@@ -4362,8 +4405,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="47"/>
-      <c r="B36" s="33"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
         <v>85</v>
@@ -4373,8 +4416,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="47"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5" t="s">
         <v>86</v>
@@ -4384,8 +4427,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="47"/>
-      <c r="B38" s="34"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5" t="s">
         <v>87</v>
@@ -4393,7 +4436,7 @@
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="47"/>
+      <c r="A39" s="33"/>
       <c r="B39" s="6" t="s">
         <v>51</v>
       </c>
@@ -4408,8 +4451,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="47"/>
-      <c r="B40" s="35"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6" t="s">
         <v>98</v>
@@ -4419,8 +4462,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="47"/>
-      <c r="B41" s="36"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="48"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6" t="s">
         <v>99</v>
@@ -4430,8 +4473,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="47"/>
-      <c r="B42" s="36"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6" t="s">
         <v>100</v>
@@ -4441,8 +4484,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="47"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6" t="s">
         <v>101</v>
@@ -4452,8 +4495,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="47"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6" t="s">
         <v>102</v>
@@ -4463,8 +4506,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="47"/>
-      <c r="B45" s="37"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="49"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6" t="s">
         <v>103</v>
@@ -4474,7 +4517,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="47"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="7" t="s">
         <v>24</v>
       </c>
@@ -4489,8 +4532,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="47"/>
-      <c r="B47" s="29"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="41"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7" t="s">
         <v>113</v>
@@ -4500,8 +4543,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="47"/>
-      <c r="B48" s="30"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="42"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7" t="s">
         <v>114</v>
@@ -4511,8 +4554,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="47"/>
-      <c r="B49" s="30"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="42"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7" t="s">
         <v>115</v>
@@ -4522,8 +4565,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="47"/>
-      <c r="B50" s="30"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="42"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7" t="s">
         <v>116</v>
@@ -4533,8 +4576,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="47"/>
-      <c r="B51" s="30"/>
+      <c r="A51" s="33"/>
+      <c r="B51" s="42"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7" t="s">
         <v>117</v>
@@ -4544,8 +4587,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="47"/>
-      <c r="B52" s="30"/>
+      <c r="A52" s="33"/>
+      <c r="B52" s="42"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7" t="s">
         <v>118</v>
@@ -4555,8 +4598,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="47"/>
-      <c r="B53" s="30"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="42"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7" t="s">
         <v>119</v>
@@ -4564,8 +4607,8 @@
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="47"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="33"/>
+      <c r="B54" s="43"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7" t="s">
         <v>120</v>
@@ -4573,7 +4616,7 @@
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="47"/>
+      <c r="A55" s="33"/>
       <c r="B55" s="8" t="s">
         <v>128</v>
       </c>
@@ -4588,8 +4631,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="47"/>
-      <c r="B56" s="44"/>
+      <c r="A56" s="33"/>
+      <c r="B56" s="37"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8" t="s">
         <v>131</v>
@@ -4599,8 +4642,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="47"/>
-      <c r="B57" s="45"/>
+      <c r="A57" s="33"/>
+      <c r="B57" s="38"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8" t="s">
         <v>132</v>
@@ -4610,8 +4653,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="47"/>
-      <c r="B58" s="45"/>
+      <c r="A58" s="33"/>
+      <c r="B58" s="38"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8" t="s">
         <v>133</v>
@@ -4621,8 +4664,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="47"/>
-      <c r="B59" s="45"/>
+      <c r="A59" s="33"/>
+      <c r="B59" s="38"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8" t="s">
         <v>134</v>
@@ -4632,8 +4675,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="47"/>
-      <c r="B60" s="46"/>
+      <c r="A60" s="33"/>
+      <c r="B60" s="39"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8" t="s">
@@ -4641,7 +4684,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="47"/>
+      <c r="A61" s="33"/>
       <c r="B61" s="9" t="s">
         <v>13</v>
       </c>
@@ -4656,8 +4699,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="47"/>
-      <c r="B62" s="38"/>
+      <c r="A62" s="33"/>
+      <c r="B62" s="29"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9" t="s">
         <v>143</v>
@@ -4667,8 +4710,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="47"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="33"/>
+      <c r="B63" s="30"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9" t="s">
         <v>144</v>
@@ -4678,8 +4721,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="47"/>
-      <c r="B64" s="39"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="30"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9" t="s">
         <v>145</v>
@@ -4689,8 +4732,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="47"/>
-      <c r="B65" s="39"/>
+      <c r="A65" s="33"/>
+      <c r="B65" s="30"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9" t="s">
         <v>146</v>
@@ -4700,8 +4743,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="47"/>
-      <c r="B66" s="39"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9" t="s">
         <v>147</v>
@@ -4709,8 +4752,8 @@
       <c r="E66" s="9"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="47"/>
-      <c r="B67" s="39"/>
+      <c r="A67" s="33"/>
+      <c r="B67" s="30"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9" t="s">
         <v>148</v>
@@ -4718,8 +4761,8 @@
       <c r="E67" s="9"/>
     </row>
     <row r="68" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="47"/>
-      <c r="B68" s="40"/>
+      <c r="A68" s="33"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
         <v>149</v>
@@ -4747,7 +4790,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="50" t="s">
         <v>238</v>
       </c>
       <c r="B70" s="7" t="s">
@@ -4767,8 +4810,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="42"/>
-      <c r="B71" s="29"/>
+      <c r="A71" s="51"/>
+      <c r="B71" s="41"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7" t="s">
         <v>170</v>
@@ -4781,8 +4824,8 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="42"/>
-      <c r="B72" s="30"/>
+      <c r="A72" s="51"/>
+      <c r="B72" s="42"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7" t="s">
         <v>171</v>
@@ -4795,8 +4838,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="42"/>
-      <c r="B73" s="30"/>
+      <c r="A73" s="51"/>
+      <c r="B73" s="42"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7" t="s">
         <v>172</v>
@@ -4809,8 +4852,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="42"/>
-      <c r="B74" s="30"/>
+      <c r="A74" s="51"/>
+      <c r="B74" s="42"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7" t="s">
         <v>173</v>
@@ -4821,8 +4864,8 @@
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="42"/>
-      <c r="B75" s="31"/>
+      <c r="A75" s="51"/>
+      <c r="B75" s="43"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7" t="s">
         <v>174</v>
@@ -4833,7 +4876,7 @@
       <c r="F75" s="7"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="42"/>
+      <c r="A76" s="51"/>
       <c r="B76" s="6" t="s">
         <v>51</v>
       </c>
@@ -4851,8 +4894,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="42"/>
-      <c r="B77" s="35"/>
+      <c r="A77" s="51"/>
+      <c r="B77" s="47"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6" t="s">
         <v>187</v>
@@ -4865,8 +4908,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="42"/>
-      <c r="B78" s="36"/>
+      <c r="A78" s="51"/>
+      <c r="B78" s="48"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6" t="s">
         <v>188</v>
@@ -4879,8 +4922,8 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="42"/>
-      <c r="B79" s="36"/>
+      <c r="A79" s="51"/>
+      <c r="B79" s="48"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6" t="s">
         <v>189</v>
@@ -4891,8 +4934,8 @@
       <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="42"/>
-      <c r="B80" s="36"/>
+      <c r="A80" s="51"/>
+      <c r="B80" s="48"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6" t="s">
         <v>190</v>
@@ -4903,8 +4946,8 @@
       <c r="F80" s="6"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="42"/>
-      <c r="B81" s="36"/>
+      <c r="A81" s="51"/>
+      <c r="B81" s="48"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6" t="s">
         <v>191</v>
@@ -4915,8 +4958,8 @@
       <c r="F81" s="6"/>
     </row>
     <row r="82" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="42"/>
-      <c r="B82" s="37"/>
+      <c r="A82" s="51"/>
+      <c r="B82" s="49"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
         <v>192</v>
@@ -4927,7 +4970,7 @@
       <c r="F82" s="6"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="42"/>
+      <c r="A83" s="51"/>
       <c r="B83" s="5" t="s">
         <v>39</v>
       </c>
@@ -4945,8 +4988,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="42"/>
-      <c r="B84" s="32"/>
+      <c r="A84" s="51"/>
+      <c r="B84" s="44"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5" t="s">
         <v>203</v>
@@ -4959,8 +5002,8 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="42"/>
-      <c r="B85" s="33"/>
+      <c r="A85" s="51"/>
+      <c r="B85" s="45"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5" t="s">
         <v>204</v>
@@ -4973,8 +5016,8 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="42"/>
-      <c r="B86" s="33"/>
+      <c r="A86" s="51"/>
+      <c r="B86" s="45"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5" t="s">
         <v>26</v>
@@ -4987,8 +5030,8 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="42"/>
-      <c r="B87" s="34"/>
+      <c r="A87" s="51"/>
+      <c r="B87" s="46"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5" t="s">
         <v>205</v>
@@ -4999,7 +5042,7 @@
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="42"/>
+      <c r="A88" s="51"/>
       <c r="B88" s="9" t="s">
         <v>158</v>
       </c>
@@ -5017,8 +5060,8 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="42"/>
-      <c r="B89" s="38"/>
+      <c r="A89" s="51"/>
+      <c r="B89" s="29"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9" t="s">
         <v>216</v>
@@ -5031,8 +5074,8 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="42"/>
-      <c r="B90" s="39"/>
+      <c r="A90" s="51"/>
+      <c r="B90" s="30"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9" t="s">
         <v>217</v>
@@ -5045,8 +5088,8 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="42"/>
-      <c r="B91" s="39"/>
+      <c r="A91" s="51"/>
+      <c r="B91" s="30"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9" t="s">
         <v>1</v>
@@ -5057,8 +5100,8 @@
       <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="42"/>
-      <c r="B92" s="40"/>
+      <c r="A92" s="51"/>
+      <c r="B92" s="31"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9" t="s">
         <v>218</v>
@@ -5069,7 +5112,7 @@
       <c r="F92" s="9"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="42"/>
+      <c r="A93" s="51"/>
       <c r="B93" s="8" t="s">
         <v>65</v>
       </c>
@@ -5087,8 +5130,8 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="42"/>
-      <c r="B94" s="44"/>
+      <c r="A94" s="51"/>
+      <c r="B94" s="37"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8" t="s">
         <v>227</v>
@@ -5101,8 +5144,8 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="42"/>
-      <c r="B95" s="45"/>
+      <c r="A95" s="51"/>
+      <c r="B95" s="38"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8" t="s">
         <v>53</v>
@@ -5115,8 +5158,8 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="42"/>
-      <c r="B96" s="45"/>
+      <c r="A96" s="51"/>
+      <c r="B96" s="38"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8" t="s">
         <v>228</v>
@@ -5127,8 +5170,8 @@
       <c r="F96" s="8"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="42"/>
-      <c r="B97" s="45"/>
+      <c r="A97" s="51"/>
+      <c r="B97" s="38"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
         <v>229</v>
@@ -5139,8 +5182,8 @@
       <c r="F97" s="8"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="43"/>
-      <c r="B98" s="46"/>
+      <c r="A98" s="52"/>
+      <c r="B98" s="39"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8" t="s">
         <v>56</v>
@@ -5165,7 +5208,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="48" t="s">
+      <c r="A100" s="36" t="s">
         <v>156</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -5179,7 +5222,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="48"/>
+      <c r="A101" s="36"/>
       <c r="B101" s="5" t="s">
         <v>39</v>
       </c>
@@ -5191,7 +5234,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="48"/>
+      <c r="A102" s="36"/>
       <c r="B102" s="9" t="s">
         <v>70</v>
       </c>
@@ -5203,7 +5246,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="48"/>
+      <c r="A103" s="36"/>
       <c r="B103" s="6" t="s">
         <v>74</v>
       </c>
@@ -5215,7 +5258,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="48"/>
+      <c r="A104" s="36"/>
       <c r="B104" s="7" t="s">
         <v>24</v>
       </c>
@@ -5238,7 +5281,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="48" t="s">
+      <c r="A106" s="36" t="s">
         <v>79</v>
       </c>
       <c r="B106" s="8" t="s">
@@ -5249,7 +5292,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="48"/>
+      <c r="A107" s="36"/>
       <c r="B107" s="5" t="s">
         <v>39</v>
       </c>
@@ -5258,7 +5301,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="48"/>
+      <c r="A108" s="36"/>
       <c r="B108" s="9" t="s">
         <v>158</v>
       </c>
@@ -5267,7 +5310,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="48"/>
+      <c r="A109" s="36"/>
       <c r="B109" s="6" t="s">
         <v>51</v>
       </c>
@@ -5276,7 +5319,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="48"/>
+      <c r="A110" s="36"/>
       <c r="B110" s="7" t="s">
         <v>24</v>
       </c>
@@ -5304,11 +5347,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A2:A29"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="A100:A104"/>
     <mergeCell ref="A106:A110"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B20:B23"/>
@@ -5324,10 +5362,469 @@
     <mergeCell ref="B89:B92"/>
     <mergeCell ref="B94:B98"/>
     <mergeCell ref="A31:A68"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A2:A29"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="A100:A104"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{51904EFB-172E-6D43-9258-28322C0BC6B3}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268E9011-BD39-6842-9E7A-20FAC21AED27}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:A87"/>
+  <sheetViews>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -6204,8 +6701,8 @@
   </sheetPr>
   <dimension ref="A1:A96"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A96" sqref="A1:A96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6703,8 +7200,8 @@
   </sheetPr>
   <dimension ref="A1:A94"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7899,8 +8396,8 @@
   </sheetPr>
   <dimension ref="A1:A150"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection sqref="A1:A150"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A163" sqref="A154:A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8662,13 +9159,102 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3FD261-3C1A-1A44-B872-867814A905FF}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2E38B7-8964-344E-BF0C-B4600A5334A6}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:A216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+    <sheetView topLeftCell="A192" workbookViewId="0">
       <selection activeCell="I225" sqref="I225"/>
     </sheetView>
   </sheetViews>
@@ -9758,458 +10344,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268E9011-BD39-6842-9E7A-20FAC21AED27}">
-  <sheetPr>
-    <tabColor theme="2" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:A87"/>
-  <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>554</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>